<commit_message>
Update Session 04 - Part 2
</commit_message>
<xml_diff>
--- a/Homeworks/Database Design & Questions.xlsx
+++ b/Homeworks/Database Design & Questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tonywoo/GitHub/Aptech/nodejs-tutorials/Homeworks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FF5524-F66B-DC48-82F4-393CBF5A17EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2D3407-37A1-C74F-BA87-D5F96B768A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PHẦN I Tables" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="177">
   <si>
     <t>No.</t>
   </si>
@@ -179,12 +179,6 @@
   </si>
   <si>
     <t>Reference Employees (Id)</t>
-  </si>
-  <si>
-    <t>OrderId</t>
-  </si>
-  <si>
-    <t>Reference Orders (Id)</t>
   </si>
   <si>
     <t>ProductId</t>
@@ -578,7 +572,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -682,6 +676,12 @@
       <color rgb="FF0070C0"/>
       <name val="Cambria"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -903,7 +903,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1233,6 +1233,14 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1259,14 +1267,7 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1286,7 +1287,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1574,7 +1575,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1585,10 +1586,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:Z900"/>
+  <dimension ref="A2:Z899"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="219" zoomScaleNormal="219" workbookViewId="0">
+      <selection activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1608,7 +1609,7 @@
     <row r="2" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="101" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1637,7 +1638,7 @@
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="80" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B3" s="80"/>
       <c r="C3" s="80"/>
@@ -1719,7 +1720,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="6"/>
@@ -1757,7 +1758,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D6" s="7">
         <v>50</v>
@@ -1795,7 +1796,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D7" s="7">
         <v>500</v>
@@ -1826,22 +1827,22 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" s="103" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="155">
+      <c r="A8" s="145">
         <v>4</v>
       </c>
-      <c r="B8" s="155" t="s">
+      <c r="B8" s="145" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="146" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" s="145"/>
+      <c r="E8" s="146"/>
+      <c r="F8" s="145"/>
+      <c r="G8" s="145"/>
+      <c r="H8" s="145"/>
+      <c r="I8" s="145" t="s">
         <v>129</v>
-      </c>
-      <c r="C8" s="156" t="s">
-        <v>130</v>
-      </c>
-      <c r="D8" s="155"/>
-      <c r="E8" s="156"/>
-      <c r="F8" s="155"/>
-      <c r="G8" s="155"/>
-      <c r="H8" s="155"/>
-      <c r="I8" s="155" t="s">
-        <v>131</v>
       </c>
       <c r="J8" s="102"/>
       <c r="K8" s="102"/>
@@ -1862,21 +1863,21 @@
       <c r="Z8" s="102"/>
     </row>
     <row r="9" spans="1:26" s="103" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="157">
+      <c r="A9" s="147">
         <v>5</v>
       </c>
-      <c r="B9" s="157" t="s">
-        <v>136</v>
-      </c>
-      <c r="C9" s="158" t="s">
-        <v>103</v>
-      </c>
-      <c r="D9" s="157"/>
-      <c r="E9" s="158"/>
-      <c r="F9" s="157"/>
-      <c r="G9" s="157"/>
-      <c r="H9" s="157"/>
-      <c r="I9" s="157"/>
+      <c r="B9" s="147" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="148" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="147"/>
+      <c r="E9" s="148"/>
+      <c r="F9" s="147"/>
+      <c r="G9" s="147"/>
+      <c r="H9" s="147"/>
+      <c r="I9" s="147"/>
       <c r="J9" s="102"/>
       <c r="K9" s="102"/>
       <c r="L9" s="102"/>
@@ -1896,21 +1897,21 @@
       <c r="Z9" s="102"/>
     </row>
     <row r="10" spans="1:26" s="103" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="157">
+      <c r="A10" s="147">
         <v>6</v>
       </c>
-      <c r="B10" s="157" t="s">
-        <v>124</v>
-      </c>
-      <c r="C10" s="158" t="s">
-        <v>125</v>
-      </c>
-      <c r="D10" s="157"/>
-      <c r="E10" s="158"/>
-      <c r="F10" s="157"/>
-      <c r="G10" s="157"/>
-      <c r="H10" s="157"/>
-      <c r="I10" s="157"/>
+      <c r="B10" s="147" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="148" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" s="147"/>
+      <c r="E10" s="148"/>
+      <c r="F10" s="147"/>
+      <c r="G10" s="147"/>
+      <c r="H10" s="147"/>
+      <c r="I10" s="147"/>
       <c r="J10" s="102"/>
       <c r="K10" s="102"/>
       <c r="L10" s="102"/>
@@ -1959,7 +1960,7 @@
     </row>
     <row r="12" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="97" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B12" s="97"/>
       <c r="C12" s="97"/>
@@ -2041,7 +2042,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="14"/>
@@ -2079,7 +2080,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D15" s="17">
         <v>100</v>
@@ -2115,7 +2116,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D16" s="17">
         <v>50</v>
@@ -2153,7 +2154,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D17" s="17">
         <v>50</v>
@@ -2193,7 +2194,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D18" s="17">
         <v>500</v>
@@ -2250,17 +2251,17 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="150" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" s="150"/>
-      <c r="C20" s="150"/>
-      <c r="D20" s="150"/>
-      <c r="E20" s="150"/>
-      <c r="F20" s="150"/>
-      <c r="G20" s="150"/>
-      <c r="H20" s="150"/>
-      <c r="I20" s="150"/>
+      <c r="A20" s="154" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="154"/>
+      <c r="C20" s="154"/>
+      <c r="D20" s="154"/>
+      <c r="E20" s="154"/>
+      <c r="F20" s="154"/>
+      <c r="G20" s="154"/>
+      <c r="H20" s="154"/>
+      <c r="I20" s="154"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -2333,7 +2334,7 @@
         <v>9</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D22" s="24">
         <v>50</v>
@@ -2371,7 +2372,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D23" s="28">
         <v>50</v>
@@ -2407,7 +2408,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D24" s="28">
         <v>50</v>
@@ -2443,7 +2444,7 @@
         <v>17</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D25" s="28">
         <v>50</v>
@@ -2481,7 +2482,7 @@
         <v>18</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D26" s="28">
         <v>500</v>
@@ -2519,7 +2520,7 @@
         <v>16</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D27" s="28">
         <v>50</v>
@@ -2614,17 +2615,17 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="147" t="s">
-        <v>98</v>
-      </c>
-      <c r="B30" s="148"/>
-      <c r="C30" s="148"/>
-      <c r="D30" s="148"/>
-      <c r="E30" s="148"/>
-      <c r="F30" s="148"/>
-      <c r="G30" s="148"/>
-      <c r="H30" s="148"/>
-      <c r="I30" s="149"/>
+      <c r="A30" s="151" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" s="152"/>
+      <c r="C30" s="152"/>
+      <c r="D30" s="152"/>
+      <c r="E30" s="152"/>
+      <c r="F30" s="152"/>
+      <c r="G30" s="152"/>
+      <c r="H30" s="152"/>
+      <c r="I30" s="153"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -2697,7 +2698,7 @@
         <v>9</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D32" s="32">
         <v>50</v>
@@ -2735,7 +2736,7 @@
         <v>19</v>
       </c>
       <c r="C33" s="35" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D33" s="36">
         <v>50</v>
@@ -2771,7 +2772,7 @@
         <v>20</v>
       </c>
       <c r="C34" s="35" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D34" s="36">
         <v>50</v>
@@ -2807,7 +2808,7 @@
         <v>17</v>
       </c>
       <c r="C35" s="35" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D35" s="36">
         <v>50</v>
@@ -2845,7 +2846,7 @@
         <v>18</v>
       </c>
       <c r="C36" s="35" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D36" s="36">
         <v>500</v>
@@ -2883,7 +2884,7 @@
         <v>16</v>
       </c>
       <c r="C37" s="35" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D37" s="36">
         <v>50</v>
@@ -2978,17 +2979,17 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="151" t="s">
-        <v>99</v>
-      </c>
-      <c r="B40" s="151"/>
-      <c r="C40" s="151"/>
-      <c r="D40" s="151"/>
-      <c r="E40" s="151"/>
-      <c r="F40" s="151"/>
-      <c r="G40" s="151"/>
-      <c r="H40" s="151"/>
-      <c r="I40" s="151"/>
+      <c r="A40" s="155" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="155"/>
+      <c r="C40" s="155"/>
+      <c r="D40" s="155"/>
+      <c r="E40" s="155"/>
+      <c r="F40" s="155"/>
+      <c r="G40" s="155"/>
+      <c r="H40" s="155"/>
+      <c r="I40" s="155"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
@@ -3061,7 +3062,7 @@
         <v>9</v>
       </c>
       <c r="C42" s="40" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D42" s="41"/>
       <c r="E42" s="42"/>
@@ -3099,7 +3100,7 @@
         <v>12</v>
       </c>
       <c r="C43" s="44" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D43" s="45">
         <v>50</v>
@@ -3182,7 +3183,7 @@
         <v>0</v>
       </c>
       <c r="H45" s="43" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I45" s="43"/>
       <c r="J45" s="1"/>
@@ -3247,7 +3248,7 @@
         <v>28</v>
       </c>
       <c r="C47" s="110" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D47" s="111"/>
       <c r="E47" s="112"/>
@@ -3285,7 +3286,7 @@
         <v>31</v>
       </c>
       <c r="C48" s="110" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D48" s="111"/>
       <c r="E48" s="112"/>
@@ -3323,7 +3324,7 @@
         <v>14</v>
       </c>
       <c r="C49" s="115" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D49" s="116" t="s">
         <v>33</v>
@@ -3356,10 +3357,10 @@
         <v>9</v>
       </c>
       <c r="B50" s="104" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C50" s="105" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D50" s="106"/>
       <c r="E50" s="105"/>
@@ -3367,7 +3368,7 @@
       <c r="G50" s="104"/>
       <c r="H50" s="107"/>
       <c r="I50" s="104" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J50" s="102"/>
       <c r="K50" s="102"/>
@@ -3392,10 +3393,10 @@
         <v>10</v>
       </c>
       <c r="B51" s="104" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C51" s="108" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D51" s="106"/>
       <c r="E51" s="105"/>
@@ -3426,10 +3427,10 @@
         <v>11</v>
       </c>
       <c r="B52" s="104" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C52" s="105" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D52" s="106"/>
       <c r="E52" s="105"/>
@@ -3437,7 +3438,7 @@
       <c r="G52" s="104"/>
       <c r="H52" s="107"/>
       <c r="I52" s="104" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J52" s="102"/>
       <c r="K52" s="102"/>
@@ -3486,13 +3487,13 @@
       <c r="Z53" s="1"/>
     </row>
     <row r="54" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="152" t="s">
-        <v>100</v>
-      </c>
-      <c r="B54" s="153"/>
-      <c r="C54" s="153"/>
-      <c r="D54" s="153"/>
-      <c r="E54" s="153"/>
+      <c r="A54" s="156" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54" s="157"/>
+      <c r="C54" s="157"/>
+      <c r="D54" s="157"/>
+      <c r="E54" s="157"/>
       <c r="F54" s="50"/>
       <c r="G54" s="50"/>
       <c r="H54" s="50"/>
@@ -3569,7 +3570,7 @@
         <v>9</v>
       </c>
       <c r="C56" s="53" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D56" s="54"/>
       <c r="E56" s="55"/>
@@ -3683,7 +3684,7 @@
         <v>38</v>
       </c>
       <c r="C59" s="57" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D59" s="61">
         <v>50</v>
@@ -3723,7 +3724,7 @@
         <v>14</v>
       </c>
       <c r="C60" s="57" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D60" s="61" t="s">
         <v>33</v>
@@ -3761,7 +3762,7 @@
         <v>41</v>
       </c>
       <c r="C61" s="57" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D61" s="61">
         <v>500</v>
@@ -3797,7 +3798,7 @@
         <v>42</v>
       </c>
       <c r="C62" s="57" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D62" s="61">
         <v>20</v>
@@ -3808,7 +3809,7 @@
         <v>43</v>
       </c>
       <c r="H62" s="56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I62" s="56"/>
       <c r="J62" s="1"/>
@@ -3829,95 +3830,95 @@
       <c r="Y62" s="1"/>
       <c r="Z62" s="1"/>
     </row>
-    <row r="63" spans="1:26" s="103" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="118">
+    <row r="63" spans="1:26" s="159" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="56">
         <v>8</v>
       </c>
-      <c r="B63" s="118" t="s">
+      <c r="B63" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="C63" s="119" t="s">
-        <v>102</v>
-      </c>
-      <c r="D63" s="120">
+      <c r="C63" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="D63" s="61">
         <v>50</v>
       </c>
-      <c r="E63" s="121"/>
-      <c r="F63" s="122" t="s">
+      <c r="E63" s="62"/>
+      <c r="F63" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="G63" s="118"/>
-      <c r="H63" s="118" t="s">
+      <c r="G63" s="56"/>
+      <c r="H63" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="I63" s="118"/>
-      <c r="J63" s="102"/>
-      <c r="K63" s="102"/>
-      <c r="L63" s="102"/>
-      <c r="M63" s="102"/>
-      <c r="N63" s="102"/>
-      <c r="O63" s="102"/>
-      <c r="P63" s="102"/>
-      <c r="Q63" s="102"/>
-      <c r="R63" s="102"/>
-      <c r="S63" s="102"/>
-      <c r="T63" s="102"/>
-      <c r="U63" s="102"/>
-      <c r="V63" s="102"/>
-      <c r="W63" s="102"/>
-      <c r="X63" s="102"/>
-      <c r="Y63" s="102"/>
-      <c r="Z63" s="102"/>
-    </row>
-    <row r="64" spans="1:26" s="103" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="118">
+      <c r="I63" s="56"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="1"/>
+      <c r="S63" s="1"/>
+      <c r="T63" s="1"/>
+      <c r="U63" s="1"/>
+      <c r="V63" s="1"/>
+      <c r="W63" s="1"/>
+      <c r="X63" s="1"/>
+      <c r="Y63" s="1"/>
+      <c r="Z63" s="1"/>
+    </row>
+    <row r="64" spans="1:26" s="159" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="56">
         <v>9</v>
       </c>
-      <c r="B64" s="118" t="s">
+      <c r="B64" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="C64" s="119" t="s">
-        <v>102</v>
-      </c>
-      <c r="D64" s="120">
+      <c r="C64" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="D64" s="61">
         <v>50</v>
       </c>
-      <c r="E64" s="121"/>
-      <c r="F64" s="122" t="s">
+      <c r="E64" s="62"/>
+      <c r="F64" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="G64" s="118"/>
-      <c r="H64" s="118" t="s">
+      <c r="G64" s="56"/>
+      <c r="H64" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="I64" s="118"/>
-      <c r="J64" s="102"/>
-      <c r="K64" s="102"/>
-      <c r="L64" s="102"/>
-      <c r="M64" s="102"/>
-      <c r="N64" s="102"/>
-      <c r="O64" s="102"/>
-      <c r="P64" s="102"/>
-      <c r="Q64" s="102"/>
-      <c r="R64" s="102"/>
-      <c r="S64" s="102"/>
-      <c r="T64" s="102"/>
-      <c r="U64" s="102"/>
-      <c r="V64" s="102"/>
-      <c r="W64" s="102"/>
-      <c r="X64" s="102"/>
-      <c r="Y64" s="102"/>
-      <c r="Z64" s="102"/>
+      <c r="I64" s="56"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="1"/>
+      <c r="S64" s="1"/>
+      <c r="T64" s="1"/>
+      <c r="U64" s="1"/>
+      <c r="V64" s="1"/>
+      <c r="W64" s="1"/>
+      <c r="X64" s="1"/>
+      <c r="Y64" s="1"/>
+      <c r="Z64" s="1"/>
     </row>
     <row r="65" spans="1:26" s="103" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="118">
         <v>10</v>
       </c>
       <c r="B65" s="118" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C65" s="119" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D65" s="120"/>
       <c r="E65" s="121"/>
@@ -3948,10 +3949,10 @@
         <v>12</v>
       </c>
       <c r="B66" s="118" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C66" s="119" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D66" s="120"/>
       <c r="E66" s="121"/>
@@ -3982,10 +3983,10 @@
         <v>13</v>
       </c>
       <c r="B67" s="118" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C67" s="119" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D67" s="120"/>
       <c r="E67" s="121"/>
@@ -4040,13 +4041,13 @@
       <c r="Z68" s="1"/>
     </row>
     <row r="69" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="154" t="s">
-        <v>101</v>
-      </c>
-      <c r="B69" s="153"/>
-      <c r="C69" s="153"/>
-      <c r="D69" s="153"/>
-      <c r="E69" s="153"/>
+      <c r="A69" s="158" t="s">
+        <v>99</v>
+      </c>
+      <c r="B69" s="157"/>
+      <c r="C69" s="157"/>
+      <c r="D69" s="157"/>
+      <c r="E69" s="157"/>
       <c r="F69" s="63"/>
       <c r="G69" s="63"/>
       <c r="H69" s="50"/>
@@ -4123,7 +4124,7 @@
         <v>9</v>
       </c>
       <c r="C71" s="124" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D71" s="125"/>
       <c r="E71" s="126"/>
@@ -4155,13 +4156,13 @@
     </row>
     <row r="72" spans="1:26" s="103" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="129">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B72" s="129" t="s">
         <v>48</v>
       </c>
       <c r="C72" s="130" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D72" s="131"/>
       <c r="E72" s="132"/>
@@ -4193,23 +4194,19 @@
     </row>
     <row r="73" spans="1:26" s="103" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="129">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B73" s="129" t="s">
         <v>50</v>
       </c>
       <c r="C73" s="130" t="s">
-        <v>102</v>
+        <v>26</v>
       </c>
       <c r="D73" s="131"/>
       <c r="E73" s="132"/>
-      <c r="F73" s="129" t="s">
-        <v>29</v>
-      </c>
+      <c r="F73" s="129"/>
       <c r="G73" s="129"/>
-      <c r="H73" s="118" t="s">
-        <v>51</v>
-      </c>
+      <c r="H73" s="118"/>
       <c r="I73" s="129"/>
       <c r="J73" s="102"/>
       <c r="K73" s="102"/>
@@ -4231,10 +4228,10 @@
     </row>
     <row r="74" spans="1:26" s="103" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="129">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B74" s="129" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="C74" s="130" t="s">
         <v>26</v>
@@ -4265,13 +4262,13 @@
     </row>
     <row r="75" spans="1:26" s="103" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="129">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B75" s="129" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C75" s="130" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="D75" s="131"/>
       <c r="E75" s="132"/>
@@ -4297,50 +4294,46 @@
       <c r="Y75" s="102"/>
       <c r="Z75" s="102"/>
     </row>
-    <row r="76" spans="1:26" s="103" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="129">
-        <v>6</v>
-      </c>
-      <c r="B76" s="129" t="s">
-        <v>25</v>
-      </c>
-      <c r="C76" s="130" t="s">
-        <v>104</v>
-      </c>
-      <c r="D76" s="131"/>
-      <c r="E76" s="132"/>
-      <c r="F76" s="129"/>
-      <c r="G76" s="129"/>
-      <c r="H76" s="118"/>
-      <c r="I76" s="129"/>
-      <c r="J76" s="102"/>
-      <c r="K76" s="102"/>
-      <c r="L76" s="102"/>
-      <c r="M76" s="102"/>
-      <c r="N76" s="102"/>
-      <c r="O76" s="102"/>
-      <c r="P76" s="102"/>
-      <c r="Q76" s="102"/>
-      <c r="R76" s="102"/>
-      <c r="S76" s="102"/>
-      <c r="T76" s="102"/>
-      <c r="U76" s="102"/>
-      <c r="V76" s="102"/>
-      <c r="W76" s="102"/>
-      <c r="X76" s="102"/>
-      <c r="Y76" s="102"/>
-      <c r="Z76" s="102"/>
+    <row r="76" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="A76" s="65"/>
+      <c r="B76" s="65"/>
+      <c r="C76" s="65"/>
+      <c r="D76" s="65"/>
+      <c r="E76" s="65"/>
+      <c r="F76" s="65"/>
+      <c r="G76" s="65"/>
+      <c r="H76" s="65"/>
+      <c r="I76" s="65"/>
+      <c r="J76" s="65"/>
+      <c r="K76" s="65"/>
+      <c r="L76" s="65"/>
+      <c r="M76" s="65"/>
+      <c r="N76" s="65"/>
+      <c r="O76" s="65"/>
+      <c r="P76" s="65"/>
+      <c r="Q76" s="65"/>
+      <c r="R76" s="65"/>
+      <c r="S76" s="65"/>
+      <c r="T76" s="65"/>
+      <c r="U76" s="65"/>
+      <c r="V76" s="65"/>
+      <c r="W76" s="65"/>
+      <c r="X76" s="65"/>
+      <c r="Y76" s="65"/>
+      <c r="Z76" s="65"/>
     </row>
     <row r="77" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" s="65"/>
-      <c r="B77" s="65"/>
-      <c r="C77" s="65"/>
-      <c r="D77" s="65"/>
-      <c r="E77" s="65"/>
-      <c r="F77" s="65"/>
-      <c r="G77" s="65"/>
-      <c r="H77" s="65"/>
-      <c r="I77" s="65"/>
+      <c r="A77" s="149" t="s">
+        <v>115</v>
+      </c>
+      <c r="B77" s="150"/>
+      <c r="C77" s="150"/>
+      <c r="D77" s="150"/>
+      <c r="E77" s="150"/>
+      <c r="F77" s="82"/>
+      <c r="G77" s="82"/>
+      <c r="H77" s="81"/>
+      <c r="I77" s="82"/>
       <c r="J77" s="65"/>
       <c r="K77" s="65"/>
       <c r="L77" s="65"/>
@@ -4360,17 +4353,33 @@
       <c r="Z77" s="65"/>
     </row>
     <row r="78" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A78" s="145" t="s">
-        <v>117</v>
-      </c>
-      <c r="B78" s="146"/>
-      <c r="C78" s="146"/>
-      <c r="D78" s="146"/>
-      <c r="E78" s="146"/>
-      <c r="F78" s="82"/>
-      <c r="G78" s="82"/>
-      <c r="H78" s="81"/>
-      <c r="I78" s="82"/>
+      <c r="A78" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" s="83" t="s">
+        <v>2</v>
+      </c>
+      <c r="D78" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="E78" s="83" t="s">
+        <v>4</v>
+      </c>
+      <c r="F78" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="G78" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="H78" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="I78" s="83" t="s">
+        <v>8</v>
+      </c>
       <c r="J78" s="65"/>
       <c r="K78" s="65"/>
       <c r="L78" s="65"/>
@@ -4390,33 +4399,25 @@
       <c r="Z78" s="65"/>
     </row>
     <row r="79" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="B79" s="83" t="s">
+      <c r="A79" s="85">
         <v>1</v>
       </c>
-      <c r="C79" s="83" t="s">
-        <v>2</v>
-      </c>
-      <c r="D79" s="83" t="s">
-        <v>3</v>
-      </c>
-      <c r="E79" s="83" t="s">
-        <v>4</v>
-      </c>
-      <c r="F79" s="83" t="s">
-        <v>5</v>
-      </c>
-      <c r="G79" s="83" t="s">
-        <v>6</v>
-      </c>
-      <c r="H79" s="84" t="s">
-        <v>7</v>
-      </c>
-      <c r="I79" s="83" t="s">
-        <v>8</v>
-      </c>
+      <c r="B79" s="85" t="s">
+        <v>9</v>
+      </c>
+      <c r="C79" s="86" t="s">
+        <v>100</v>
+      </c>
+      <c r="D79" s="87"/>
+      <c r="E79" s="88"/>
+      <c r="F79" s="89" t="s">
+        <v>10</v>
+      </c>
+      <c r="G79" s="89"/>
+      <c r="H79" s="90" t="s">
+        <v>11</v>
+      </c>
+      <c r="I79" s="89"/>
       <c r="J79" s="65"/>
       <c r="K79" s="65"/>
       <c r="L79" s="65"/>
@@ -4435,56 +4436,54 @@
       <c r="Y79" s="65"/>
       <c r="Z79" s="65"/>
     </row>
-    <row r="80" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A80" s="85">
-        <v>1</v>
-      </c>
-      <c r="B80" s="85" t="s">
-        <v>9</v>
-      </c>
-      <c r="C80" s="86" t="s">
-        <v>102</v>
-      </c>
-      <c r="D80" s="87"/>
-      <c r="E80" s="88"/>
-      <c r="F80" s="89" t="s">
-        <v>10</v>
-      </c>
-      <c r="G80" s="89"/>
-      <c r="H80" s="90" t="s">
-        <v>11</v>
-      </c>
-      <c r="I80" s="89"/>
-      <c r="J80" s="65"/>
-      <c r="K80" s="65"/>
-      <c r="L80" s="65"/>
-      <c r="M80" s="65"/>
-      <c r="N80" s="65"/>
-      <c r="O80" s="65"/>
-      <c r="P80" s="65"/>
-      <c r="Q80" s="65"/>
-      <c r="R80" s="65"/>
-      <c r="S80" s="65"/>
-      <c r="T80" s="65"/>
-      <c r="U80" s="65"/>
-      <c r="V80" s="65"/>
-      <c r="W80" s="65"/>
-      <c r="X80" s="65"/>
-      <c r="Y80" s="65"/>
-      <c r="Z80" s="65"/>
+    <row r="80" spans="1:26" s="103" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A80" s="133">
+        <v>2</v>
+      </c>
+      <c r="B80" s="133" t="s">
+        <v>116</v>
+      </c>
+      <c r="C80" s="134" t="s">
+        <v>101</v>
+      </c>
+      <c r="D80" s="135"/>
+      <c r="E80" s="136"/>
+      <c r="F80" s="133"/>
+      <c r="G80" s="133"/>
+      <c r="H80" s="137"/>
+      <c r="I80" s="133"/>
+      <c r="J80" s="138"/>
+      <c r="K80" s="138"/>
+      <c r="L80" s="138"/>
+      <c r="M80" s="138"/>
+      <c r="N80" s="138"/>
+      <c r="O80" s="138"/>
+      <c r="P80" s="138"/>
+      <c r="Q80" s="138"/>
+      <c r="R80" s="138"/>
+      <c r="S80" s="138"/>
+      <c r="T80" s="138"/>
+      <c r="U80" s="138"/>
+      <c r="V80" s="138"/>
+      <c r="W80" s="138"/>
+      <c r="X80" s="138"/>
+      <c r="Y80" s="138"/>
+      <c r="Z80" s="138"/>
     </row>
     <row r="81" spans="1:26" s="103" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="133">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B81" s="133" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C81" s="134" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D81" s="135"/>
-      <c r="E81" s="136"/>
+      <c r="E81" s="136" t="s">
+        <v>119</v>
+      </c>
       <c r="F81" s="133"/>
       <c r="G81" s="133"/>
       <c r="H81" s="137"/>
@@ -4509,18 +4508,16 @@
     </row>
     <row r="82" spans="1:26" s="103" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="133">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B82" s="133" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C82" s="134" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D82" s="135"/>
-      <c r="E82" s="136" t="s">
-        <v>121</v>
-      </c>
+      <c r="E82" s="136"/>
       <c r="F82" s="133"/>
       <c r="G82" s="133"/>
       <c r="H82" s="137"/>
@@ -4545,13 +4542,13 @@
     </row>
     <row r="83" spans="1:26" s="103" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="133">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B83" s="133" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C83" s="134" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D83" s="135"/>
       <c r="E83" s="136"/>
@@ -4579,20 +4576,22 @@
     </row>
     <row r="84" spans="1:26" s="103" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="133">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B84" s="133" t="s">
+        <v>122</v>
+      </c>
+      <c r="C84" s="134" t="s">
         <v>123</v>
-      </c>
-      <c r="C84" s="134" t="s">
-        <v>103</v>
       </c>
       <c r="D84" s="135"/>
       <c r="E84" s="136"/>
       <c r="F84" s="133"/>
       <c r="G84" s="133"/>
       <c r="H84" s="137"/>
-      <c r="I84" s="133"/>
+      <c r="I84" s="133" t="s">
+        <v>124</v>
+      </c>
       <c r="J84" s="138"/>
       <c r="K84" s="138"/>
       <c r="L84" s="138"/>
@@ -4613,22 +4612,20 @@
     </row>
     <row r="85" spans="1:26" s="103" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="133">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B85" s="133" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C85" s="134" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D85" s="135"/>
       <c r="E85" s="136"/>
       <c r="F85" s="133"/>
       <c r="G85" s="133"/>
       <c r="H85" s="137"/>
-      <c r="I85" s="133" t="s">
-        <v>126</v>
-      </c>
+      <c r="I85" s="133"/>
       <c r="J85" s="138"/>
       <c r="K85" s="138"/>
       <c r="L85" s="138"/>
@@ -4647,50 +4644,46 @@
       <c r="Y85" s="138"/>
       <c r="Z85" s="138"/>
     </row>
-    <row r="86" spans="1:26" s="103" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A86" s="133">
-        <v>7</v>
-      </c>
-      <c r="B86" s="133" t="s">
-        <v>127</v>
-      </c>
-      <c r="C86" s="134" t="s">
-        <v>128</v>
-      </c>
-      <c r="D86" s="135"/>
-      <c r="E86" s="136"/>
-      <c r="F86" s="133"/>
-      <c r="G86" s="133"/>
-      <c r="H86" s="137"/>
-      <c r="I86" s="133"/>
-      <c r="J86" s="138"/>
-      <c r="K86" s="138"/>
-      <c r="L86" s="138"/>
-      <c r="M86" s="138"/>
-      <c r="N86" s="138"/>
-      <c r="O86" s="138"/>
-      <c r="P86" s="138"/>
-      <c r="Q86" s="138"/>
-      <c r="R86" s="138"/>
-      <c r="S86" s="138"/>
-      <c r="T86" s="138"/>
-      <c r="U86" s="138"/>
-      <c r="V86" s="138"/>
-      <c r="W86" s="138"/>
-      <c r="X86" s="138"/>
-      <c r="Y86" s="138"/>
-      <c r="Z86" s="138"/>
+    <row r="86" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+      <c r="K86" s="1"/>
+      <c r="L86" s="1"/>
+      <c r="M86" s="1"/>
+      <c r="N86" s="1"/>
+      <c r="O86" s="1"/>
+      <c r="P86" s="1"/>
+      <c r="Q86" s="1"/>
+      <c r="R86" s="1"/>
+      <c r="S86" s="1"/>
+      <c r="T86" s="1"/>
+      <c r="U86" s="1"/>
+      <c r="V86" s="1"/>
+      <c r="W86" s="1"/>
+      <c r="X86" s="1"/>
+      <c r="Y86" s="1"/>
+      <c r="Z86" s="1"/>
     </row>
     <row r="87" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1"/>
-      <c r="I87" s="1"/>
+      <c r="A87" s="149" t="s">
+        <v>120</v>
+      </c>
+      <c r="B87" s="150"/>
+      <c r="C87" s="150"/>
+      <c r="D87" s="150"/>
+      <c r="E87" s="150"/>
+      <c r="F87" s="82"/>
+      <c r="G87" s="82"/>
+      <c r="H87" s="81"/>
+      <c r="I87" s="82"/>
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
       <c r="L87" s="1"/>
@@ -4710,17 +4703,33 @@
       <c r="Z87" s="1"/>
     </row>
     <row r="88" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="145" t="s">
-        <v>122</v>
-      </c>
-      <c r="B88" s="146"/>
-      <c r="C88" s="146"/>
-      <c r="D88" s="146"/>
-      <c r="E88" s="146"/>
-      <c r="F88" s="82"/>
-      <c r="G88" s="82"/>
-      <c r="H88" s="81"/>
-      <c r="I88" s="82"/>
+      <c r="A88" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="B88" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="C88" s="83" t="s">
+        <v>2</v>
+      </c>
+      <c r="D88" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="E88" s="83" t="s">
+        <v>4</v>
+      </c>
+      <c r="F88" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="G88" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="H88" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="I88" s="83" t="s">
+        <v>8</v>
+      </c>
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
       <c r="L88" s="1"/>
@@ -4739,72 +4748,60 @@
       <c r="Y88" s="1"/>
       <c r="Z88" s="1"/>
     </row>
-    <row r="89" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="B89" s="83" t="s">
+    <row r="89" spans="1:26" s="103" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="139">
         <v>1</v>
       </c>
-      <c r="C89" s="83" t="s">
+      <c r="B89" s="139" t="s">
+        <v>9</v>
+      </c>
+      <c r="C89" s="140" t="s">
+        <v>100</v>
+      </c>
+      <c r="D89" s="141"/>
+      <c r="E89" s="142"/>
+      <c r="F89" s="143" t="s">
+        <v>10</v>
+      </c>
+      <c r="G89" s="143"/>
+      <c r="H89" s="144" t="s">
+        <v>11</v>
+      </c>
+      <c r="I89" s="143"/>
+      <c r="J89" s="102"/>
+      <c r="K89" s="102"/>
+      <c r="L89" s="102"/>
+      <c r="M89" s="102"/>
+      <c r="N89" s="102"/>
+      <c r="O89" s="102"/>
+      <c r="P89" s="102"/>
+      <c r="Q89" s="102"/>
+      <c r="R89" s="102"/>
+      <c r="S89" s="102"/>
+      <c r="T89" s="102"/>
+      <c r="U89" s="102"/>
+      <c r="V89" s="102"/>
+      <c r="W89" s="102"/>
+      <c r="X89" s="102"/>
+      <c r="Y89" s="102"/>
+      <c r="Z89" s="102"/>
+    </row>
+    <row r="90" spans="1:26" s="103" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="133">
         <v>2</v>
       </c>
-      <c r="D89" s="83" t="s">
-        <v>3</v>
-      </c>
-      <c r="E89" s="83" t="s">
-        <v>4</v>
-      </c>
-      <c r="F89" s="83" t="s">
-        <v>5</v>
-      </c>
-      <c r="G89" s="83" t="s">
-        <v>6</v>
-      </c>
-      <c r="H89" s="84" t="s">
-        <v>7</v>
-      </c>
-      <c r="I89" s="83" t="s">
-        <v>8</v>
-      </c>
-      <c r="J89" s="1"/>
-      <c r="K89" s="1"/>
-      <c r="L89" s="1"/>
-      <c r="M89" s="1"/>
-      <c r="N89" s="1"/>
-      <c r="O89" s="1"/>
-      <c r="P89" s="1"/>
-      <c r="Q89" s="1"/>
-      <c r="R89" s="1"/>
-      <c r="S89" s="1"/>
-      <c r="T89" s="1"/>
-      <c r="U89" s="1"/>
-      <c r="V89" s="1"/>
-      <c r="W89" s="1"/>
-      <c r="X89" s="1"/>
-      <c r="Y89" s="1"/>
-      <c r="Z89" s="1"/>
-    </row>
-    <row r="90" spans="1:26" s="103" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="139">
-        <v>1</v>
-      </c>
-      <c r="B90" s="139" t="s">
-        <v>9</v>
-      </c>
-      <c r="C90" s="140" t="s">
-        <v>102</v>
-      </c>
-      <c r="D90" s="141"/>
-      <c r="E90" s="142"/>
-      <c r="F90" s="143" t="s">
-        <v>10</v>
-      </c>
-      <c r="G90" s="143"/>
-      <c r="H90" s="144" t="s">
-        <v>11</v>
-      </c>
-      <c r="I90" s="143"/>
+      <c r="B90" s="133" t="s">
+        <v>116</v>
+      </c>
+      <c r="C90" s="134" t="s">
+        <v>101</v>
+      </c>
+      <c r="D90" s="135"/>
+      <c r="E90" s="136"/>
+      <c r="F90" s="133"/>
+      <c r="G90" s="133"/>
+      <c r="H90" s="137"/>
+      <c r="I90" s="133"/>
       <c r="J90" s="102"/>
       <c r="K90" s="102"/>
       <c r="L90" s="102"/>
@@ -4825,16 +4822,18 @@
     </row>
     <row r="91" spans="1:26" s="103" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="133">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B91" s="133" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C91" s="134" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D91" s="135"/>
-      <c r="E91" s="136"/>
+      <c r="E91" s="136" t="s">
+        <v>119</v>
+      </c>
       <c r="F91" s="133"/>
       <c r="G91" s="133"/>
       <c r="H91" s="137"/>
@@ -4859,18 +4858,16 @@
     </row>
     <row r="92" spans="1:26" s="103" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="133">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B92" s="133" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C92" s="134" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D92" s="135"/>
-      <c r="E92" s="136" t="s">
-        <v>121</v>
-      </c>
+      <c r="E92" s="136"/>
       <c r="F92" s="133"/>
       <c r="G92" s="133"/>
       <c r="H92" s="137"/>
@@ -4895,13 +4892,13 @@
     </row>
     <row r="93" spans="1:26" s="103" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="133">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B93" s="133" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C93" s="134" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D93" s="135"/>
       <c r="E93" s="136"/>
@@ -4929,20 +4926,22 @@
     </row>
     <row r="94" spans="1:26" s="103" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="133">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B94" s="133" t="s">
+        <v>122</v>
+      </c>
+      <c r="C94" s="134" t="s">
         <v>123</v>
-      </c>
-      <c r="C94" s="134" t="s">
-        <v>103</v>
       </c>
       <c r="D94" s="135"/>
       <c r="E94" s="136"/>
       <c r="F94" s="133"/>
       <c r="G94" s="133"/>
       <c r="H94" s="137"/>
-      <c r="I94" s="133"/>
+      <c r="I94" s="133" t="s">
+        <v>124</v>
+      </c>
       <c r="J94" s="102"/>
       <c r="K94" s="102"/>
       <c r="L94" s="102"/>
@@ -4961,56 +4960,56 @@
       <c r="Y94" s="102"/>
       <c r="Z94" s="102"/>
     </row>
-    <row r="95" spans="1:26" s="103" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:26" s="103" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="133">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B95" s="133" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C95" s="134" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D95" s="135"/>
       <c r="E95" s="136"/>
       <c r="F95" s="133"/>
       <c r="G95" s="133"/>
       <c r="H95" s="137"/>
-      <c r="I95" s="133" t="s">
-        <v>126</v>
-      </c>
-      <c r="J95" s="102"/>
-      <c r="K95" s="102"/>
-      <c r="L95" s="102"/>
-      <c r="M95" s="102"/>
-      <c r="N95" s="102"/>
-      <c r="O95" s="102"/>
-      <c r="P95" s="102"/>
-      <c r="Q95" s="102"/>
-      <c r="R95" s="102"/>
-      <c r="S95" s="102"/>
-      <c r="T95" s="102"/>
-      <c r="U95" s="102"/>
-      <c r="V95" s="102"/>
-      <c r="W95" s="102"/>
-      <c r="X95" s="102"/>
-      <c r="Y95" s="102"/>
-      <c r="Z95" s="102"/>
+      <c r="I95" s="133"/>
+      <c r="J95" s="138"/>
+      <c r="K95" s="138"/>
+      <c r="L95" s="138"/>
+      <c r="M95" s="138"/>
+      <c r="N95" s="138"/>
+      <c r="O95" s="138"/>
+      <c r="P95" s="138"/>
+      <c r="Q95" s="138"/>
+      <c r="R95" s="138"/>
+      <c r="S95" s="138"/>
+      <c r="T95" s="138"/>
+      <c r="U95" s="138"/>
+      <c r="V95" s="138"/>
+      <c r="W95" s="138"/>
+      <c r="X95" s="138"/>
+      <c r="Y95" s="138"/>
+      <c r="Z95" s="138"/>
     </row>
     <row r="96" spans="1:26" s="103" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="133">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B96" s="133" t="s">
-        <v>127</v>
+        <v>34</v>
       </c>
       <c r="C96" s="134" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="D96" s="135"/>
       <c r="E96" s="136"/>
       <c r="F96" s="133"/>
-      <c r="G96" s="133"/>
+      <c r="G96" s="133" t="s">
+        <v>172</v>
+      </c>
       <c r="H96" s="137"/>
       <c r="I96" s="133"/>
       <c r="J96" s="138"/>
@@ -5032,21 +5031,17 @@
       <c r="Z96" s="138"/>
     </row>
     <row r="97" spans="1:26" s="103" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A97" s="133">
-        <v>8</v>
-      </c>
+      <c r="A97" s="133"/>
       <c r="B97" s="133" t="s">
-        <v>34</v>
+        <v>173</v>
       </c>
       <c r="C97" s="134" t="s">
-        <v>151</v>
+        <v>100</v>
       </c>
       <c r="D97" s="135"/>
       <c r="E97" s="136"/>
       <c r="F97" s="133"/>
-      <c r="G97" s="133" t="s">
-        <v>174</v>
-      </c>
+      <c r="G97" s="133"/>
       <c r="H97" s="137"/>
       <c r="I97" s="133"/>
       <c r="J97" s="138"/>
@@ -5070,10 +5065,10 @@
     <row r="98" spans="1:26" s="103" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="133"/>
       <c r="B98" s="133" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C98" s="134" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
       <c r="D98" s="135"/>
       <c r="E98" s="136"/>
@@ -5102,10 +5097,10 @@
     <row r="99" spans="1:26" s="103" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="133"/>
       <c r="B99" s="133" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C99" s="134" t="s">
-        <v>151</v>
+        <v>100</v>
       </c>
       <c r="D99" s="135"/>
       <c r="E99" s="136"/>
@@ -5134,10 +5129,10 @@
     <row r="100" spans="1:26" s="103" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="133"/>
       <c r="B100" s="133" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C100" s="134" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="D100" s="135"/>
       <c r="E100" s="136"/>
@@ -5163,48 +5158,46 @@
       <c r="Y100" s="138"/>
       <c r="Z100" s="138"/>
     </row>
-    <row r="101" spans="1:26" s="103" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A101" s="133"/>
-      <c r="B101" s="133" t="s">
-        <v>178</v>
-      </c>
-      <c r="C101" s="134" t="s">
-        <v>128</v>
-      </c>
-      <c r="D101" s="135"/>
-      <c r="E101" s="136"/>
-      <c r="F101" s="133"/>
-      <c r="G101" s="133"/>
-      <c r="H101" s="137"/>
-      <c r="I101" s="133"/>
-      <c r="J101" s="138"/>
-      <c r="K101" s="138"/>
-      <c r="L101" s="138"/>
-      <c r="M101" s="138"/>
-      <c r="N101" s="138"/>
-      <c r="O101" s="138"/>
-      <c r="P101" s="138"/>
-      <c r="Q101" s="138"/>
-      <c r="R101" s="138"/>
-      <c r="S101" s="138"/>
-      <c r="T101" s="138"/>
-      <c r="U101" s="138"/>
-      <c r="V101" s="138"/>
-      <c r="W101" s="138"/>
-      <c r="X101" s="138"/>
-      <c r="Y101" s="138"/>
-      <c r="Z101" s="138"/>
+    <row r="101" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+      <c r="J101" s="1"/>
+      <c r="K101" s="1"/>
+      <c r="L101" s="1"/>
+      <c r="M101" s="1"/>
+      <c r="N101" s="1"/>
+      <c r="O101" s="1"/>
+      <c r="P101" s="1"/>
+      <c r="Q101" s="1"/>
+      <c r="R101" s="1"/>
+      <c r="S101" s="1"/>
+      <c r="T101" s="1"/>
+      <c r="U101" s="1"/>
+      <c r="V101" s="1"/>
+      <c r="W101" s="1"/>
+      <c r="X101" s="1"/>
+      <c r="Y101" s="1"/>
+      <c r="Z101" s="1"/>
     </row>
     <row r="102" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
-      <c r="E102" s="1"/>
-      <c r="F102" s="1"/>
-      <c r="G102" s="1"/>
-      <c r="H102" s="1"/>
-      <c r="I102" s="1"/>
+      <c r="A102" s="149" t="s">
+        <v>139</v>
+      </c>
+      <c r="B102" s="150"/>
+      <c r="C102" s="150"/>
+      <c r="D102" s="150"/>
+      <c r="E102" s="150"/>
+      <c r="F102" s="82"/>
+      <c r="G102" s="82"/>
+      <c r="H102" s="81"/>
+      <c r="I102" s="82"/>
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
       <c r="L102" s="1"/>
@@ -5224,17 +5217,33 @@
       <c r="Z102" s="1"/>
     </row>
     <row r="103" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="145" t="s">
-        <v>141</v>
-      </c>
-      <c r="B103" s="146"/>
-      <c r="C103" s="146"/>
-      <c r="D103" s="146"/>
-      <c r="E103" s="146"/>
-      <c r="F103" s="82"/>
-      <c r="G103" s="82"/>
-      <c r="H103" s="81"/>
-      <c r="I103" s="82"/>
+      <c r="A103" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="B103" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="C103" s="83" t="s">
+        <v>2</v>
+      </c>
+      <c r="D103" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="E103" s="83" t="s">
+        <v>4</v>
+      </c>
+      <c r="F103" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="G103" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="H103" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="I103" s="83" t="s">
+        <v>8</v>
+      </c>
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
       <c r="L103" s="1"/>
@@ -5253,72 +5262,62 @@
       <c r="Y103" s="1"/>
       <c r="Z103" s="1"/>
     </row>
-    <row r="104" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="B104" s="83" t="s">
+    <row r="104" spans="1:26" s="103" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="139">
         <v>1</v>
       </c>
-      <c r="C104" s="83" t="s">
+      <c r="B104" s="139" t="s">
+        <v>9</v>
+      </c>
+      <c r="C104" s="140" t="s">
+        <v>100</v>
+      </c>
+      <c r="D104" s="141"/>
+      <c r="E104" s="142"/>
+      <c r="F104" s="143" t="s">
+        <v>10</v>
+      </c>
+      <c r="G104" s="143"/>
+      <c r="H104" s="144" t="s">
+        <v>11</v>
+      </c>
+      <c r="I104" s="143"/>
+      <c r="J104" s="102"/>
+      <c r="K104" s="102"/>
+      <c r="L104" s="102"/>
+      <c r="M104" s="102"/>
+      <c r="N104" s="102"/>
+      <c r="O104" s="102"/>
+      <c r="P104" s="102"/>
+      <c r="Q104" s="102"/>
+      <c r="R104" s="102"/>
+      <c r="S104" s="102"/>
+      <c r="T104" s="102"/>
+      <c r="U104" s="102"/>
+      <c r="V104" s="102"/>
+      <c r="W104" s="102"/>
+      <c r="X104" s="102"/>
+      <c r="Y104" s="102"/>
+      <c r="Z104" s="102"/>
+    </row>
+    <row r="105" spans="1:26" s="103" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="133">
         <v>2</v>
       </c>
-      <c r="D104" s="83" t="s">
-        <v>3</v>
-      </c>
-      <c r="E104" s="83" t="s">
-        <v>4</v>
-      </c>
-      <c r="F104" s="83" t="s">
-        <v>5</v>
-      </c>
-      <c r="G104" s="83" t="s">
-        <v>6</v>
-      </c>
-      <c r="H104" s="84" t="s">
-        <v>7</v>
-      </c>
-      <c r="I104" s="83" t="s">
-        <v>8</v>
-      </c>
-      <c r="J104" s="1"/>
-      <c r="K104" s="1"/>
-      <c r="L104" s="1"/>
-      <c r="M104" s="1"/>
-      <c r="N104" s="1"/>
-      <c r="O104" s="1"/>
-      <c r="P104" s="1"/>
-      <c r="Q104" s="1"/>
-      <c r="R104" s="1"/>
-      <c r="S104" s="1"/>
-      <c r="T104" s="1"/>
-      <c r="U104" s="1"/>
-      <c r="V104" s="1"/>
-      <c r="W104" s="1"/>
-      <c r="X104" s="1"/>
-      <c r="Y104" s="1"/>
-      <c r="Z104" s="1"/>
-    </row>
-    <row r="105" spans="1:26" s="103" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="139">
-        <v>1</v>
-      </c>
-      <c r="B105" s="139" t="s">
-        <v>9</v>
-      </c>
-      <c r="C105" s="140" t="s">
-        <v>102</v>
-      </c>
-      <c r="D105" s="141"/>
-      <c r="E105" s="142"/>
-      <c r="F105" s="143" t="s">
-        <v>10</v>
-      </c>
-      <c r="G105" s="143"/>
-      <c r="H105" s="144" t="s">
-        <v>11</v>
-      </c>
-      <c r="I105" s="143"/>
+      <c r="B105" s="133" t="s">
+        <v>16</v>
+      </c>
+      <c r="C105" s="134" t="s">
+        <v>101</v>
+      </c>
+      <c r="D105" s="135"/>
+      <c r="E105" s="136"/>
+      <c r="F105" s="133" t="s">
+        <v>13</v>
+      </c>
+      <c r="G105" s="133"/>
+      <c r="H105" s="137"/>
+      <c r="I105" s="133"/>
       <c r="J105" s="102"/>
       <c r="K105" s="102"/>
       <c r="L105" s="102"/>
@@ -5339,19 +5338,17 @@
     </row>
     <row r="106" spans="1:26" s="103" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="133">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B106" s="133" t="s">
-        <v>16</v>
+        <v>140</v>
       </c>
       <c r="C106" s="134" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D106" s="135"/>
       <c r="E106" s="136"/>
-      <c r="F106" s="133" t="s">
-        <v>13</v>
-      </c>
+      <c r="F106" s="133"/>
       <c r="G106" s="133"/>
       <c r="H106" s="137"/>
       <c r="I106" s="133"/>
@@ -5375,13 +5372,13 @@
     </row>
     <row r="107" spans="1:26" s="103" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="133">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B107" s="133" t="s">
+        <v>141</v>
+      </c>
+      <c r="C107" s="134" t="s">
         <v>142</v>
-      </c>
-      <c r="C107" s="134" t="s">
-        <v>103</v>
       </c>
       <c r="D107" s="135"/>
       <c r="E107" s="136"/>
@@ -5409,13 +5406,13 @@
     </row>
     <row r="108" spans="1:26" s="103" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="133">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B108" s="133" t="s">
         <v>143</v>
       </c>
       <c r="C108" s="134" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="D108" s="135"/>
       <c r="E108" s="136"/>
@@ -5443,13 +5440,13 @@
     </row>
     <row r="109" spans="1:26" s="103" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="133">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B109" s="133" t="s">
+        <v>144</v>
+      </c>
+      <c r="C109" s="134" t="s">
         <v>145</v>
-      </c>
-      <c r="C109" s="134" t="s">
-        <v>128</v>
       </c>
       <c r="D109" s="135"/>
       <c r="E109" s="136"/>
@@ -5475,50 +5472,44 @@
       <c r="Y109" s="102"/>
       <c r="Z109" s="102"/>
     </row>
-    <row r="110" spans="1:26" s="103" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="133">
-        <v>6</v>
-      </c>
-      <c r="B110" s="133" t="s">
-        <v>146</v>
-      </c>
-      <c r="C110" s="134" t="s">
-        <v>147</v>
-      </c>
-      <c r="D110" s="135"/>
-      <c r="E110" s="136"/>
-      <c r="F110" s="133"/>
-      <c r="G110" s="133"/>
-      <c r="H110" s="137"/>
-      <c r="I110" s="133"/>
-      <c r="J110" s="102"/>
-      <c r="K110" s="102"/>
-      <c r="L110" s="102"/>
-      <c r="M110" s="102"/>
-      <c r="N110" s="102"/>
-      <c r="O110" s="102"/>
-      <c r="P110" s="102"/>
-      <c r="Q110" s="102"/>
-      <c r="R110" s="102"/>
-      <c r="S110" s="102"/>
-      <c r="T110" s="102"/>
-      <c r="U110" s="102"/>
-      <c r="V110" s="102"/>
-      <c r="W110" s="102"/>
-      <c r="X110" s="102"/>
-      <c r="Y110" s="102"/>
-      <c r="Z110" s="102"/>
+    <row r="110" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="91"/>
+      <c r="B110" s="91"/>
+      <c r="C110" s="92"/>
+      <c r="D110" s="93"/>
+      <c r="E110" s="94"/>
+      <c r="F110" s="91"/>
+      <c r="G110" s="91"/>
+      <c r="H110" s="95"/>
+      <c r="I110" s="91"/>
+      <c r="J110" s="1"/>
+      <c r="K110" s="1"/>
+      <c r="L110" s="1"/>
+      <c r="M110" s="1"/>
+      <c r="N110" s="1"/>
+      <c r="O110" s="1"/>
+      <c r="P110" s="1"/>
+      <c r="Q110" s="1"/>
+      <c r="R110" s="1"/>
+      <c r="S110" s="1"/>
+      <c r="T110" s="1"/>
+      <c r="U110" s="1"/>
+      <c r="V110" s="1"/>
+      <c r="W110" s="1"/>
+      <c r="X110" s="1"/>
+      <c r="Y110" s="1"/>
+      <c r="Z110" s="1"/>
     </row>
     <row r="111" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="91"/>
-      <c r="B111" s="91"/>
-      <c r="C111" s="92"/>
-      <c r="D111" s="93"/>
-      <c r="E111" s="94"/>
-      <c r="F111" s="91"/>
-      <c r="G111" s="91"/>
-      <c r="H111" s="95"/>
-      <c r="I111" s="91"/>
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1"/>
+      <c r="F111" s="1"/>
+      <c r="G111" s="1"/>
+      <c r="H111" s="1"/>
+      <c r="I111" s="1"/>
       <c r="J111" s="1"/>
       <c r="K111" s="1"/>
       <c r="L111" s="1"/>
@@ -27601,42 +27592,14 @@
       <c r="Y899" s="1"/>
       <c r="Z899" s="1"/>
     </row>
-    <row r="900" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A900" s="1"/>
-      <c r="B900" s="1"/>
-      <c r="C900" s="1"/>
-      <c r="D900" s="1"/>
-      <c r="E900" s="1"/>
-      <c r="F900" s="1"/>
-      <c r="G900" s="1"/>
-      <c r="H900" s="1"/>
-      <c r="I900" s="1"/>
-      <c r="J900" s="1"/>
-      <c r="K900" s="1"/>
-      <c r="L900" s="1"/>
-      <c r="M900" s="1"/>
-      <c r="N900" s="1"/>
-      <c r="O900" s="1"/>
-      <c r="P900" s="1"/>
-      <c r="Q900" s="1"/>
-      <c r="R900" s="1"/>
-      <c r="S900" s="1"/>
-      <c r="T900" s="1"/>
-      <c r="U900" s="1"/>
-      <c r="V900" s="1"/>
-      <c r="W900" s="1"/>
-      <c r="X900" s="1"/>
-      <c r="Y900" s="1"/>
-      <c r="Z900" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A103:E103"/>
-    <mergeCell ref="A88:E88"/>
+    <mergeCell ref="A102:E102"/>
+    <mergeCell ref="A87:E87"/>
     <mergeCell ref="A30:I30"/>
     <mergeCell ref="A20:I20"/>
     <mergeCell ref="A40:I40"/>
-    <mergeCell ref="A78:E78"/>
+    <mergeCell ref="A77:E77"/>
     <mergeCell ref="A54:E54"/>
     <mergeCell ref="A69:E69"/>
   </mergeCells>
@@ -27666,13 +27629,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="145" t="s">
-        <v>148</v>
-      </c>
-      <c r="B3" s="146"/>
-      <c r="C3" s="146"/>
-      <c r="D3" s="146"/>
-      <c r="E3" s="146"/>
+      <c r="A3" s="149" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="150"/>
+      <c r="C3" s="150"/>
+      <c r="D3" s="150"/>
+      <c r="E3" s="150"/>
       <c r="F3" s="82"/>
       <c r="G3" s="82"/>
       <c r="H3" s="81"/>
@@ -27715,7 +27678,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="86" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D5" s="87"/>
       <c r="E5" s="88"/>
@@ -27736,7 +27699,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="92" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D6" s="93"/>
       <c r="E6" s="94"/>
@@ -27752,10 +27715,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="91" t="s">
+        <v>147</v>
+      </c>
+      <c r="C7" s="92" t="s">
         <v>149</v>
-      </c>
-      <c r="C7" s="92" t="s">
-        <v>151</v>
       </c>
       <c r="D7" s="93"/>
       <c r="E7" s="94"/>
@@ -27764,7 +27727,7 @@
       <c r="H7" s="95"/>
       <c r="I7" s="91"/>
       <c r="L7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -27772,10 +27735,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="91" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C8" s="92" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D8" s="93"/>
       <c r="E8" s="94"/>
@@ -27789,10 +27752,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="91" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C9" s="92" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D9" s="93"/>
       <c r="E9" s="94"/>
@@ -27800,10 +27763,10 @@
       <c r="G9" s="91"/>
       <c r="H9" s="95"/>
       <c r="I9" s="91" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L9" s="98" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="M9" s="99"/>
     </row>
@@ -27817,10 +27780,10 @@
       <c r="G10" s="91"/>
       <c r="H10" s="95"/>
       <c r="I10" s="91" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L10" s="98" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M10" s="99"/>
     </row>
@@ -27847,36 +27810,36 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="L14" s="98" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="M14" s="99" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
+        <v>157</v>
+      </c>
+      <c r="E15" t="s">
+        <v>158</v>
+      </c>
+      <c r="F15" t="s">
         <v>159</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" t="s">
         <v>160</v>
       </c>
-      <c r="F15" t="s">
+      <c r="H15" t="s">
         <v>161</v>
       </c>
-      <c r="G15" t="s">
+      <c r="I15" t="s">
         <v>162</v>
       </c>
-      <c r="H15" t="s">
+      <c r="J15" t="s">
         <v>163</v>
       </c>
-      <c r="I15" t="s">
-        <v>164</v>
-      </c>
-      <c r="J15" t="s">
-        <v>165</v>
-      </c>
       <c r="L15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M15">
         <v>15</v>
@@ -27884,117 +27847,117 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D16" s="98" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E16" s="98" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F16" s="98" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G16" s="98" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H16" s="98" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I16" s="98" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J16" s="98" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D18" s="98" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E18" s="98" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F18" s="98" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G18" s="98" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H18" s="98" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I18" s="98" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J18" s="98" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D20" s="98" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E20" s="98" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F20" s="98" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G20" s="98" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H20" s="98" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I20" s="98" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J20" s="98" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -28024,14 +27987,14 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="66" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B1" s="67" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C1" s="68"/>
       <c r="D1" s="68" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E1" s="68"/>
       <c r="F1" s="68"/>
@@ -28061,7 +28024,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="70" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C2" s="65"/>
       <c r="D2" s="65"/>
@@ -28093,7 +28056,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="70" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C3" s="65"/>
       <c r="D3" s="65"/>
@@ -28125,7 +28088,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="70" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C4" s="65"/>
       <c r="D4" s="65"/>
@@ -28157,7 +28120,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="70" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C5" s="65"/>
       <c r="D5" s="65"/>
@@ -28189,7 +28152,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="70" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C6" s="65"/>
       <c r="D6" s="65"/>
@@ -28221,7 +28184,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="70" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C7" s="65"/>
       <c r="D7" s="65"/>
@@ -28250,10 +28213,10 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="66" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B8" s="67" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C8" s="68"/>
       <c r="D8" s="68"/>
@@ -28285,13 +28248,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="79" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" s="65" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D9" s="65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E9" s="65"/>
       <c r="F9" s="65"/>
@@ -28321,13 +28284,13 @@
         <v>2</v>
       </c>
       <c r="B10" s="79" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C10" s="65" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D10" s="65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E10" s="65"/>
       <c r="F10" s="65"/>
@@ -28357,13 +28320,13 @@
         <v>3</v>
       </c>
       <c r="B11" s="79" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" s="65" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D11" s="65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E11" s="65"/>
       <c r="F11" s="65"/>
@@ -28393,13 +28356,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="77" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C12" s="65" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D12" s="65" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E12" s="65"/>
       <c r="F12" s="65"/>
@@ -28429,13 +28392,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="77" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C13" s="65" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D13" s="65" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E13" s="65"/>
       <c r="F13" s="65"/>
@@ -28465,13 +28428,13 @@
         <v>6</v>
       </c>
       <c r="B14" s="77" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C14" s="65" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D14" s="65" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E14" s="65"/>
       <c r="F14" s="65"/>
@@ -28501,13 +28464,13 @@
         <v>7</v>
       </c>
       <c r="B15" s="74" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C15" s="65" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="65" t="s">
         <v>106</v>
-      </c>
-      <c r="D15" s="65" t="s">
-        <v>108</v>
       </c>
       <c r="E15" s="65"/>
       <c r="F15" s="65"/>
@@ -28537,13 +28500,13 @@
         <v>8</v>
       </c>
       <c r="B16" s="74" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C16" s="65" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="65" t="s">
         <v>106</v>
-      </c>
-      <c r="D16" s="65" t="s">
-        <v>108</v>
       </c>
       <c r="E16" s="65"/>
       <c r="F16" s="65"/>
@@ -28570,10 +28533,10 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="100" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B17" s="74" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C17" s="65"/>
       <c r="D17" s="65"/>
@@ -28605,13 +28568,13 @@
         <v>9</v>
       </c>
       <c r="B18" s="75" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C18" s="65" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="65" t="s">
         <v>106</v>
-      </c>
-      <c r="D18" s="65" t="s">
-        <v>108</v>
       </c>
       <c r="E18" s="65"/>
       <c r="F18" s="65"/>
@@ -28641,13 +28604,13 @@
         <v>10</v>
       </c>
       <c r="B19" s="74" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C19" s="65" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="65" t="s">
         <v>106</v>
-      </c>
-      <c r="D19" s="65" t="s">
-        <v>108</v>
       </c>
       <c r="E19" s="65"/>
       <c r="F19" s="65"/>
@@ -28677,13 +28640,13 @@
         <v>11</v>
       </c>
       <c r="B20" s="74" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C20" s="65" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" s="65" t="s">
         <v>106</v>
-      </c>
-      <c r="D20" s="65" t="s">
-        <v>108</v>
       </c>
       <c r="E20" s="65"/>
       <c r="F20" s="65"/>
@@ -28713,13 +28676,13 @@
         <v>12</v>
       </c>
       <c r="B21" s="74" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C21" s="65" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" s="65" t="s">
         <v>106</v>
-      </c>
-      <c r="D21" s="65" t="s">
-        <v>108</v>
       </c>
       <c r="E21" s="65"/>
       <c r="F21" s="65"/>
@@ -28749,13 +28712,13 @@
         <v>13</v>
       </c>
       <c r="B22" s="74" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C22" s="65" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="65" t="s">
         <v>106</v>
-      </c>
-      <c r="D22" s="65" t="s">
-        <v>108</v>
       </c>
       <c r="E22" s="65"/>
       <c r="F22" s="65"/>
@@ -28785,13 +28748,13 @@
         <v>14</v>
       </c>
       <c r="B23" s="72" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C23" s="65" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D23" s="65" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E23" s="65"/>
       <c r="F23" s="65"/>
@@ -28821,13 +28784,13 @@
         <v>15</v>
       </c>
       <c r="B24" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C24" s="65" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D24" s="65" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E24" s="65"/>
       <c r="F24" s="65"/>
@@ -28857,13 +28820,13 @@
         <v>16</v>
       </c>
       <c r="B25" s="72" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C25" s="65" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" s="65" t="s">
         <v>106</v>
-      </c>
-      <c r="D25" s="65" t="s">
-        <v>108</v>
       </c>
       <c r="E25" s="65"/>
       <c r="F25" s="65"/>
@@ -28893,13 +28856,13 @@
         <v>17</v>
       </c>
       <c r="B26" s="72" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C26" s="65" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D26" s="65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E26" s="65"/>
       <c r="F26" s="65"/>
@@ -28929,13 +28892,13 @@
         <v>18</v>
       </c>
       <c r="B27" s="72" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C27" s="65" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D27" s="65" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E27" s="65"/>
       <c r="F27" s="65"/>
@@ -28965,13 +28928,13 @@
         <v>19</v>
       </c>
       <c r="B28" s="72" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C28" s="65" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D28" s="65" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E28" s="65"/>
       <c r="F28" s="65"/>
@@ -29001,13 +28964,13 @@
         <v>20</v>
       </c>
       <c r="B29" s="72" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C29" s="65" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="65" t="s">
         <v>106</v>
-      </c>
-      <c r="D29" s="65" t="s">
-        <v>108</v>
       </c>
       <c r="E29" s="65"/>
       <c r="F29" s="65"/>
@@ -29037,7 +29000,7 @@
         <v>21</v>
       </c>
       <c r="B30" s="72" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C30" s="65"/>
       <c r="D30" s="65"/>
@@ -29069,7 +29032,7 @@
         <v>22</v>
       </c>
       <c r="B31" s="72" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C31" s="65"/>
       <c r="D31" s="65"/>
@@ -29101,7 +29064,7 @@
         <v>23</v>
       </c>
       <c r="B32" s="72" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C32" s="65"/>
       <c r="D32" s="65"/>
@@ -29133,7 +29096,7 @@
         <v>24</v>
       </c>
       <c r="B33" s="72" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C33" s="65"/>
       <c r="D33" s="65"/>
@@ -29165,13 +29128,13 @@
         <v>25</v>
       </c>
       <c r="B34" s="72" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C34" s="65" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D34" s="65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E34" s="65"/>
       <c r="F34" s="65"/>
@@ -29201,7 +29164,7 @@
         <v>26</v>
       </c>
       <c r="B35" s="72" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C35" s="65"/>
       <c r="D35" s="65"/>
@@ -29233,7 +29196,7 @@
         <v>27</v>
       </c>
       <c r="B36" s="72" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C36" s="65"/>
       <c r="D36" s="65"/>
@@ -29265,7 +29228,7 @@
         <v>28</v>
       </c>
       <c r="B37" s="72" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C37" s="65"/>
       <c r="D37" s="65"/>
@@ -29297,7 +29260,7 @@
         <v>29</v>
       </c>
       <c r="B38" s="72" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C38" s="65"/>
       <c r="D38" s="65"/>
@@ -29329,7 +29292,7 @@
         <v>30</v>
       </c>
       <c r="B39" s="72" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C39" s="65"/>
       <c r="D39" s="65"/>
@@ -29361,7 +29324,7 @@
         <v>31</v>
       </c>
       <c r="B40" s="72" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C40" s="65"/>
       <c r="D40" s="65"/>
@@ -29393,7 +29356,7 @@
         <v>32</v>
       </c>
       <c r="B41" s="72" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C41" s="65"/>
       <c r="D41" s="65"/>
@@ -29425,7 +29388,7 @@
         <v>33</v>
       </c>
       <c r="B42" s="72" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C42" s="65"/>
       <c r="D42" s="65"/>
@@ -29457,7 +29420,7 @@
         <v>34</v>
       </c>
       <c r="B43" s="72" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C43" s="65"/>
       <c r="D43" s="65"/>

</xml_diff>